<commit_message>
Update and delete file
</commit_message>
<xml_diff>
--- a/Fiverr Tumblr.xlsx
+++ b/Fiverr Tumblr.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="87">
   <si>
     <t>thatirishnerd.tumblr.com</t>
   </si>
@@ -254,6 +254,36 @@
   </si>
   <si>
     <t>Suka Suka Kita</t>
+  </si>
+  <si>
+    <t>rgdmff.tumblr.com</t>
+  </si>
+  <si>
+    <t>lastdragonlord.tumblr.com</t>
+  </si>
+  <si>
+    <t>offfffffffffthesouthernisles.tumblr.com</t>
+  </si>
+  <si>
+    <t>panphangirl.tumblr.com</t>
+  </si>
+  <si>
+    <t>typicalwelshnonsense.tumblr.com</t>
+  </si>
+  <si>
+    <t>Relakan</t>
+  </si>
+  <si>
+    <t>Last Dragon</t>
+  </si>
+  <si>
+    <t>Semangat Baru</t>
+  </si>
+  <si>
+    <t>Terlalu Indah</t>
+  </si>
+  <si>
+    <t>Aku Disini</t>
   </si>
 </sst>
 </file>
@@ -13249,10 +13279,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14171,6 +14201,121 @@
       </c>
       <c r="I36">
         <v>124</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37">
+        <v>32</v>
+      </c>
+      <c r="D37">
+        <v>98</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F37" t="s">
+        <v>82</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37" s="5">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38">
+        <v>33</v>
+      </c>
+      <c r="D38">
+        <v>98</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F38" t="s">
+        <v>83</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39">
+        <v>32</v>
+      </c>
+      <c r="D39">
+        <v>98</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F39" t="s">
+        <v>84</v>
+      </c>
+      <c r="H39">
+        <v>29</v>
+      </c>
+      <c r="I39" s="5">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>80</v>
+      </c>
+      <c r="C40">
+        <v>32</v>
+      </c>
+      <c r="D40">
+        <v>98</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F40" t="s">
+        <v>85</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41">
+        <v>32</v>
+      </c>
+      <c r="D41">
+        <v>98</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F41" t="s">
+        <v>86</v>
+      </c>
+      <c r="H41">
+        <v>16</v>
+      </c>
+      <c r="I41" s="5">
+        <v>18100</v>
       </c>
     </row>
   </sheetData>
@@ -14210,9 +14355,14 @@
     <hyperlink ref="E34" r:id="rId28"/>
     <hyperlink ref="E35" r:id="rId29"/>
     <hyperlink ref="E36" r:id="rId30"/>
+    <hyperlink ref="E37" r:id="rId31"/>
+    <hyperlink ref="E38" r:id="rId32"/>
+    <hyperlink ref="E39" r:id="rId33"/>
+    <hyperlink ref="E40" r:id="rId34"/>
+    <hyperlink ref="E41" r:id="rId35"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId36"/>
 </worksheet>
 </file>
 

</xml_diff>